<commit_message>
Add JSON export and project total MANA hours functionality
</commit_message>
<xml_diff>
--- a/backend/hackathon_proposal/HACKATHON_PROPOSAL.xlsx
+++ b/backend/hackathon_proposal/HACKATHON_PROPOSAL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FYRE" sheetId="1" state="visible" r:id="rId2"/>
@@ -780,8 +780,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table104" displayName="Table104" ref="A2:F5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table104" displayName="Table104" ref="A1:F4" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F4"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Role"/>
     <tableColumn id="2" name="Subproject"/>
@@ -794,8 +794,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1046" displayName="Table1046" ref="A2:F6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A2:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1046" displayName="Table1046" ref="A1:F5" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Role"/>
     <tableColumn id="2" name="Subproject"/>
@@ -888,7 +888,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.3"/>
@@ -1100,11 +1100,11 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.74"/>
@@ -1255,11 +1255,11 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.63"/>
@@ -1495,13 +1495,13 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="55.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="58.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.28"/>
   </cols>
@@ -1768,10 +1768,10 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.12"/>
@@ -2121,11 +2121,11 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18"/>
@@ -2576,7 +2576,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
@@ -3133,7 +3133,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
@@ -3562,13 +3562,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F6"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.42"/>
@@ -3577,24 +3577,44 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3608,13 +3628,13 @@
         <v>156</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3628,13 +3648,13 @@
         <v>156</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3648,35 +3668,16 @@
         <v>156</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3696,13 +3697,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F5"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="27.42"/>
@@ -3710,24 +3711,44 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3744,7 +3765,7 @@
         <v>166</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>20</v>
@@ -3761,35 +3782,16 @@
         <v>165</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F5" s="4" t="n">
         <v>40</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>